<commit_message>
drop time lag for temp and precip
</commit_message>
<xml_diff>
--- a/model_datamaps/dag_dhscovar_liftover.xlsx
+++ b/model_datamaps/dag_dhscovar_liftover.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/model_datamaps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53835B49-844B-474D-B6F8-274EC1BF8874}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717F9E2B-60C8-714A-BF7B-FC57560DF319}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3400" yWindow="2260" windowWidth="10000" windowHeight="12620" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
   </bookViews>
@@ -116,12 +116,6 @@
     <t>hlthdist_cont_scale_clst</t>
   </si>
   <si>
-    <t>temp_lag_cont_scale_clst</t>
-  </si>
-  <si>
-    <t>precip_lag_cont_scale_clst</t>
-  </si>
-  <si>
     <t>alt_dem_cont_scale_clst</t>
   </si>
   <si>
@@ -144,6 +138,12 @@
   </si>
   <si>
     <t>wlthrcde_fctb</t>
+  </si>
+  <si>
+    <t>temp_ann_cont_scale_clst</t>
+  </si>
+  <si>
+    <t>precip_ann_cont_scale_clst</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +549,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -602,10 +602,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -637,7 +637,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -645,7 +645,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -653,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -661,7 +661,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -669,15 +669,15 @@
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update dags to reflect new urbanicity
</commit_message>
<xml_diff>
--- a/model_datamaps/dag_dhscovar_liftover.xlsx
+++ b/model_datamaps/dag_dhscovar_liftover.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717F9E2B-60C8-714A-BF7B-FC57560DF319}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A464D1-5874-1E40-8CF3-10FBC89F7225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="2260" windowWidth="10000" windowHeight="12620" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
+    <workbookView xWindow="0" yWindow="8520" windowWidth="17260" windowHeight="18000" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>I:Housing Materials</t>
   </si>
@@ -122,9 +117,6 @@
     <t>hv106_fctb</t>
   </si>
   <si>
-    <t>urbanscore_cont_clst</t>
-  </si>
-  <si>
     <t>I:Pv18s</t>
   </si>
   <si>
@@ -144,6 +136,18 @@
   </si>
   <si>
     <t>precip_ann_cont_scale_clst</t>
+  </si>
+  <si>
+    <t>built_population_2014_cont_scale_clst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nightlights_composite_cont_scale_clst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> all_population_count_2015_cont_scale_clst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> travel_times_2015_cont_scale_clst</t>
   </si>
 </sst>
 </file>
@@ -166,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +189,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -198,11 +208,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC132DAB-6FA1-694E-95AA-6F077F799F31}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -602,10 +614,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -637,7 +649,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -645,7 +657,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -665,19 +677,43 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B22" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
urbanicity back to PCA formulation
</commit_message>
<xml_diff>
--- a/model_datamaps/dag_dhscovar_liftover.xlsx
+++ b/model_datamaps/dag_dhscovar_liftover.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A464D1-5874-1E40-8CF3-10FBC89F7225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668DA7E9-42A4-F14F-B6E1-957E7C81002B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8520" windowWidth="17260" windowHeight="18000" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>I:Housing Materials</t>
   </si>
@@ -138,16 +138,7 @@
     <t>precip_ann_cont_scale_clst</t>
   </si>
   <si>
-    <t>built_population_2014_cont_scale_clst</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nightlights_composite_cont_scale_clst</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> all_population_count_2015_cont_scale_clst</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> travel_times_2015_cont_scale_clst</t>
+    <t>urbanscore_cont_scale_clst</t>
   </si>
 </sst>
 </file>
@@ -529,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC132DAB-6FA1-694E-95AA-6F077F799F31}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B21"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,34 +676,10 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
major overhaul for weights -- final
</commit_message>
<xml_diff>
--- a/model_datamaps/dag_dhscovar_liftover.xlsx
+++ b/model_datamaps/dag_dhscovar_liftover.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE37D054-3853-8245-8840-9EEBC42B6D35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AC1BD6-B840-7B4E-85E9-6874FE05F6CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="1560" windowWidth="14240" windowHeight="12980" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
+    <workbookView xWindow="780" yWindow="2700" windowWidth="14240" windowHeight="12980" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,42 +98,21 @@
     <t>alt_dem_cont_scale_clst</t>
   </si>
   <si>
-    <t>hv106_fctb</t>
-  </si>
-  <si>
     <t>I:Pv18s</t>
   </si>
   <si>
     <t>Pv18s</t>
   </si>
   <si>
-    <t>I:Owns Livestock</t>
-  </si>
-  <si>
-    <t>hv246_fctb</t>
-  </si>
-  <si>
-    <t>wlthrcde_fctb</t>
-  </si>
-  <si>
     <t>wtrdist_cont_log_scale_clst</t>
   </si>
   <si>
     <t>anyatm_cont_logit_scale_clst</t>
   </si>
   <si>
-    <t>lowhb_fctb</t>
-  </si>
-  <si>
-    <t>I:Hemoglobin</t>
-  </si>
-  <si>
     <t>urban_rura_fctb</t>
   </si>
   <si>
-    <t>hlthst_nrst_duration_fctb_clst</t>
-  </si>
-  <si>
     <t>precip_mean_cont_scale_clst</t>
   </si>
   <si>
@@ -144,6 +123,27 @@
   </si>
   <si>
     <t>C:Hospital Distance</t>
+  </si>
+  <si>
+    <t>hlthdist_cont_log_scale_clst</t>
+  </si>
+  <si>
+    <t>I:Anemia</t>
+  </si>
+  <si>
+    <t>hab57_fctb</t>
+  </si>
+  <si>
+    <t>wlthrcde_combscor_cont</t>
+  </si>
+  <si>
+    <t>hv108_cont_scale</t>
+  </si>
+  <si>
+    <t>I:Farmer</t>
+  </si>
+  <si>
+    <t>farmer_fctb</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,7 +564,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -593,10 +593,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -617,10 +617,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -633,10 +633,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -644,7 +644,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -652,15 +652,15 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -676,7 +676,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -684,15 +684,15 @@
         <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean up old issues in covar and temperature
</commit_message>
<xml_diff>
--- a/model_datamaps/dag_dhscovar_liftover.xlsx
+++ b/model_datamaps/dag_dhscovar_liftover.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AC1BD6-B840-7B4E-85E9-6874FE05F6CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA62C138-BC35-1B45-ABFD-A33510B5F926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="2700" windowWidth="14240" windowHeight="12980" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>I:Housing Materials</t>
   </si>
@@ -114,12 +114,6 @@
   </si>
   <si>
     <t>precip_mean_cont_scale_clst</t>
-  </si>
-  <si>
-    <t>temp_mean_cont_scale_clst</t>
-  </si>
-  <si>
-    <t>C:Temperature</t>
   </si>
   <si>
     <t>C:Hospital Distance</t>
@@ -531,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC132DAB-6FA1-694E-95AA-6F077F799F31}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,7 +558,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -593,10 +587,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -617,10 +611,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -633,10 +627,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -657,41 +651,33 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>21</v>
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
+      <c r="A17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update for dag without anemia and antimalarials
</commit_message>
<xml_diff>
--- a/model_datamaps/dag_dhscovar_liftover.xlsx
+++ b/model_datamaps/dag_dhscovar_liftover.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA62C138-BC35-1B45-ABFD-A33510B5F926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D196BDA-3B4E-9A4D-824C-2DDECFF29DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="2700" windowWidth="14240" windowHeight="12980" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
+    <workbookView xWindow="0" yWindow="2720" windowWidth="14240" windowHeight="12980" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,14 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>I:Housing Materials</t>
   </si>
   <si>
-    <t>C:Antimalarial Use</t>
-  </si>
-  <si>
     <t>I:HIV Status</t>
   </si>
   <si>
@@ -104,12 +101,6 @@
     <t>Pv18s</t>
   </si>
   <si>
-    <t>wtrdist_cont_log_scale_clst</t>
-  </si>
-  <si>
-    <t>anyatm_cont_logit_scale_clst</t>
-  </si>
-  <si>
     <t>urban_rura_fctb</t>
   </si>
   <si>
@@ -119,15 +110,6 @@
     <t>C:Hospital Distance</t>
   </si>
   <si>
-    <t>hlthdist_cont_log_scale_clst</t>
-  </si>
-  <si>
-    <t>I:Anemia</t>
-  </si>
-  <si>
-    <t>hab57_fctb</t>
-  </si>
-  <si>
     <t>wlthrcde_combscor_cont</t>
   </si>
   <si>
@@ -138,6 +120,12 @@
   </si>
   <si>
     <t>farmer_fctb</t>
+  </si>
+  <si>
+    <t>hlthst_duration_fctb_clst</t>
+  </si>
+  <si>
+    <t>wtrdist_fctb_clst</t>
   </si>
 </sst>
 </file>
@@ -525,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC132DAB-6FA1-694E-95AA-6F077F799F31}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,10 +527,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -550,23 +538,23 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>25</v>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -587,50 +575,50 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -638,47 +626,31 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B16" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update weights and edu
</commit_message>
<xml_diff>
--- a/model_datamaps/dag_dhscovar_liftover.xlsx
+++ b/model_datamaps/dag_dhscovar_liftover.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D196BDA-3B4E-9A4D-824C-2DDECFF29DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65519F18-9BFE-1340-A256-6722952B9397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2720" windowWidth="14240" windowHeight="12980" xr2:uid="{FF80736B-9930-494E-A19E-DAA29A670E08}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>wlthrcde_combscor_cont</t>
   </si>
   <si>
-    <t>hv108_cont_scale</t>
-  </si>
-  <si>
     <t>I:Farmer</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>wtrdist_fctb_clst</t>
+  </si>
+  <si>
+    <t>hv106_fctb</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,10 +583,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -602,7 +602,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -610,7 +610,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -634,7 +634,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>